<commit_message>
2nd. Don't work logLevel FINE. Why?
</commit_message>
<xml_diff>
--- a/target/classes/StatisticsOutput.xlsx
+++ b/target/classes/StatisticsOutput.xlsx
@@ -41,16 +41,16 @@
     <t>Казанский Университет Вычислений;</t>
   </si>
   <si>
+    <t>MEDICINE</t>
+  </si>
+  <si>
+    <t>Самарский Медицинский Институт;Московский Государственный Медицинский Университет;Тамбовский Университет Медицины;</t>
+  </si>
+  <si>
     <t>PHYSICS</t>
   </si>
   <si>
     <t>Московский Придуманный Институт;Московский Выдуманный Университет;</t>
-  </si>
-  <si>
-    <t>MEDICINE</t>
-  </si>
-  <si>
-    <t>Самарский Медицинский Институт;Московский Государственный Медицинский Университет;Тамбовский Университет Медицины;</t>
   </si>
 </sst>
 </file>
@@ -183,13 +183,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>4.539999961853027</v>
+        <v>4.329999923706055</v>
       </c>
       <c r="C4" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -200,13 +200,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>4.329999923706055</v>
+        <v>4.539999961853027</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="D5" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>

</xml_diff>